<commit_message>
Moves and renames for clarity, TC summary.
</commit_message>
<xml_diff>
--- a/LDMP/data/CarbonSummaryTable.xlsx
+++ b/LDMP/data/CarbonSummaryTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azvol\Code\LandDegradation\trends.earth\LDMP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B4B815-AA72-47D5-9EDC-F942349A1DE2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAF4D36-6893-4FCC-A79D-AD515861C988}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>The boundaries, names, and designations used in this report do not imply official endorsement or acceptance by Conservation International Foundation, or its partner organizations and contributors.  This report is available under the terms of Creative Commons Attribution 4.0 International License (CC BY 4.0).</t>
   </si>
@@ -83,24 +83,43 @@
     <t>Summary of carbon change</t>
   </si>
   <si>
-    <t>Site area (hectares):</t>
-  </si>
-  <si>
     <t>Forest change over period (hectares):</t>
   </si>
   <si>
     <t>Total carbon emissions over period (tonnes of CO2 equivalent):</t>
+  </si>
+  <si>
+    <t>Percent of total land area</t>
+  </si>
+  <si>
+    <t>Area (hectares)</t>
+  </si>
+  <si>
+    <t>Forest area:</t>
+  </si>
+  <si>
+    <t>Non-forest land area:</t>
+  </si>
+  <si>
+    <t>Water area:</t>
+  </si>
+  <si>
+    <t>Missing data:</t>
+  </si>
+  <si>
+    <t>Total area:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +196,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -233,7 +260,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -273,9 +300,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -283,9 +307,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -298,19 +319,11 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="37" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -322,16 +335,45 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -662,10 +704,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H36"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +723,7 @@
     <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -688,505 +733,528 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:8" s="16" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
+    <row r="3" spans="1:6" s="16" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-    </row>
-    <row r="4" spans="1:8" s="16" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-    </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="39" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+    </row>
+    <row r="4" spans="1:6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:6" s="16" customFormat="1" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="18"/>
+    </row>
+    <row r="6" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="48"/>
+    </row>
+    <row r="7" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
+      <c r="B7" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="46"/>
+      <c r="D7" s="48"/>
+    </row>
+    <row r="8" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="46"/>
+      <c r="D8" s="48"/>
+    </row>
+    <row r="9" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="45"/>
+      <c r="D9" s="48"/>
+    </row>
+    <row r="10" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="44">
+        <f>SUM(C6:C9)</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="47"/>
+    </row>
+    <row r="11" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="40" t="s">
+      <c r="C12" s="35"/>
+      <c r="D12" s="42">
+        <f>SUM(C19:C36)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="23"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="20"/>
+      <c r="B13" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="26">
-        <f>SUM(C14:C29)</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="26">
-        <f>SUM(F13:F29)</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="24"/>
-    </row>
-    <row r="8" spans="1:8" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="24"/>
-    </row>
-    <row r="9" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
+      <c r="C13" s="35"/>
+      <c r="D13" s="42">
+        <f>SUM(F18:F36)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="23"/>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-    </row>
-    <row r="11" spans="1:8" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-    </row>
-    <row r="12" spans="1:8" s="13" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+    </row>
+    <row r="16" spans="1:6" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" s="13" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B17" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C17" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D17" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E17" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F17" s="25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28">
-        <v>2000</v>
-      </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-    </row>
-    <row r="14" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28">
-        <v>2001</v>
-      </c>
-      <c r="B14" s="29">
-        <f>B13+C14</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="31">
-        <f>D13+E14</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="32">
-        <f t="shared" ref="F14:F29" si="0">-E14*3.67</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="34"/>
-    </row>
-    <row r="15" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28">
-        <v>2002</v>
-      </c>
-      <c r="B15" s="29">
-        <f t="shared" ref="B15:B19" si="1">B14+C15</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="31">
-        <f t="shared" ref="D15:D29" si="2">D14+E15</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="33"/>
-      <c r="F15" s="32">
-        <f t="shared" ref="F15:F19" si="3">-E15*3.67</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="15"/>
-    </row>
-    <row r="16" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28">
-        <v>2003</v>
-      </c>
-      <c r="B16" s="29">
+    <row r="18" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+    </row>
+    <row r="19" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="27">
+        <f>B18+C19</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="40"/>
+      <c r="D19" s="39">
+        <f>D18+E19</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="41"/>
+      <c r="F19" s="40">
+        <f t="shared" ref="F19:F36" si="0">-E19*3.67</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="28"/>
+    </row>
+    <row r="20" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="27">
+        <f t="shared" ref="B20:B24" si="1">B19+C20</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="40"/>
+      <c r="D20" s="39">
+        <f t="shared" ref="D20:D34" si="2">D19+E20</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="41"/>
+      <c r="F20" s="40">
+        <f t="shared" ref="F20:F24" si="3">-E20*3.67</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="30"/>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="26"/>
+      <c r="B21" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="31">
+      <c r="C21" s="40"/>
+      <c r="D21" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="32">
+      <c r="E21" s="41"/>
+      <c r="F21" s="40">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H16" s="15"/>
-    </row>
-    <row r="17" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
-        <v>2004</v>
-      </c>
-      <c r="B17" s="29">
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="31">
+      <c r="C22" s="40"/>
+      <c r="D22" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E17" s="33"/>
-      <c r="F17" s="32">
+      <c r="E22" s="41"/>
+      <c r="F22" s="40">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28">
-        <v>2005</v>
-      </c>
-      <c r="B18" s="29">
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="31">
+      <c r="C23" s="40"/>
+      <c r="D23" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="32">
+      <c r="E23" s="41"/>
+      <c r="F23" s="40">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H18" s="15"/>
-    </row>
-    <row r="19" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28">
-        <v>2006</v>
-      </c>
-      <c r="B19" s="29">
+      <c r="H23" s="15"/>
+    </row>
+    <row r="24" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="26"/>
+      <c r="B24" s="27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="31">
+      <c r="C24" s="40"/>
+      <c r="D24" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="32">
+      <c r="E24" s="41"/>
+      <c r="F24" s="40">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H19" s="15"/>
-    </row>
-    <row r="20" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="28">
-        <v>2007</v>
-      </c>
-      <c r="B20" s="29">
-        <f t="shared" ref="B20:B29" si="4">B19+C20</f>
-        <v>0</v>
-      </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="31">
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="26"/>
+      <c r="B25" s="27">
+        <f t="shared" ref="B25:B34" si="4">B24+C25</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="40"/>
+      <c r="D25" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="32">
+      <c r="E25" s="41"/>
+      <c r="F25" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="15"/>
-    </row>
-    <row r="21" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="28">
-        <v>2008</v>
-      </c>
-      <c r="B21" s="29">
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="26"/>
+      <c r="B26" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="31">
+      <c r="C26" s="40"/>
+      <c r="D26" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E21" s="33"/>
-      <c r="F21" s="32">
+      <c r="E26" s="41"/>
+      <c r="F26" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H21" s="15"/>
-    </row>
-    <row r="22" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="28">
-        <v>2009</v>
-      </c>
-      <c r="B22" s="29">
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+      <c r="B27" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="31">
+      <c r="C27" s="40"/>
+      <c r="D27" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="32">
+      <c r="E27" s="41"/>
+      <c r="F27" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="15"/>
-    </row>
-    <row r="23" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28">
-        <v>2010</v>
-      </c>
-      <c r="B23" s="29">
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="40"/>
+      <c r="H28" s="15"/>
+    </row>
+    <row r="29" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="26"/>
+      <c r="B29" s="27">
+        <f>B27+C29</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="40"/>
+      <c r="D29" s="39">
+        <f>D27+E29</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="41"/>
+      <c r="F29" s="40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="15"/>
+    </row>
+    <row r="30" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="31">
+      <c r="C30" s="40"/>
+      <c r="D30" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E23" s="33"/>
-      <c r="F23" s="32">
+      <c r="E30" s="41"/>
+      <c r="F30" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H23" s="15"/>
-    </row>
-    <row r="24" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28">
-        <v>2011</v>
-      </c>
-      <c r="B24" s="29">
+      <c r="H30" s="15"/>
+    </row>
+    <row r="31" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
+      <c r="B31" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="C24" s="32"/>
-      <c r="D24" s="31">
+      <c r="C31" s="40"/>
+      <c r="D31" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E24" s="33"/>
-      <c r="F24" s="32">
+      <c r="E31" s="41"/>
+      <c r="F31" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="15"/>
-    </row>
-    <row r="25" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28">
-        <v>2012</v>
-      </c>
-      <c r="B25" s="29">
+      <c r="H31" s="15"/>
+    </row>
+    <row r="32" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="26"/>
+      <c r="B32" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="31">
+      <c r="C32" s="40"/>
+      <c r="D32" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E25" s="33"/>
-      <c r="F25" s="32">
+      <c r="E32" s="41"/>
+      <c r="F32" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H25" s="15"/>
-    </row>
-    <row r="26" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28">
-        <v>2013</v>
-      </c>
-      <c r="B26" s="29">
+      <c r="H32" s="15"/>
+    </row>
+    <row r="33" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="26"/>
+      <c r="B33" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="31">
+      <c r="C33" s="40"/>
+      <c r="D33" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E26" s="33"/>
-      <c r="F26" s="32">
+      <c r="E33" s="41"/>
+      <c r="F33" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="15"/>
-    </row>
-    <row r="27" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28">
-        <v>2014</v>
-      </c>
-      <c r="B27" s="29">
+      <c r="H33" s="15"/>
+    </row>
+    <row r="34" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="26"/>
+      <c r="B34" s="27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="31">
+      <c r="C34" s="40"/>
+      <c r="D34" s="39">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E27" s="33"/>
-      <c r="F27" s="32">
+      <c r="E34" s="41"/>
+      <c r="F34" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H27" s="15"/>
-    </row>
-    <row r="28" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="28">
-        <v>2015</v>
-      </c>
-      <c r="B28" s="29">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E28" s="33"/>
-      <c r="F28" s="32">
+      <c r="H34" s="15"/>
+    </row>
+    <row r="35" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="26"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="40"/>
+      <c r="H35" s="15"/>
+    </row>
+    <row r="36" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
+      <c r="B36" s="27">
+        <f>B34+C36</f>
+        <v>0</v>
+      </c>
+      <c r="C36" s="40"/>
+      <c r="D36" s="39">
+        <f>D34+E36</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="41"/>
+      <c r="F36" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H28" s="15"/>
-    </row>
-    <row r="29" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="28">
-        <v>2016</v>
-      </c>
-      <c r="B29" s="29">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="31">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E29" s="33"/>
-      <c r="F29" s="32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H29" s="15"/>
-    </row>
-    <row r="30" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="H30" s="15"/>
-    </row>
-    <row r="31" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
+      <c r="H36" s="15"/>
+    </row>
+    <row r="37" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="19"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="H37" s="15"/>
+    </row>
+    <row r="38" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-    </row>
-    <row r="32" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-    </row>
-    <row r="33" spans="1:6" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-    </row>
-    <row r="34" spans="1:6" s="7" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="37"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-    </row>
-    <row r="36" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="37" t="s">
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+    </row>
+    <row r="39" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+    </row>
+    <row r="40" spans="1:8" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+    </row>
+    <row r="41" spans="1:8" s="7" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+    </row>
+    <row r="43" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
+      <c r="B43" s="33"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A36:F36"/>
-    <mergeCell ref="B31:F32"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="B38:F39"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="84" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix summary table output.
</commit_message>
<xml_diff>
--- a/LDMP/data/CarbonSummaryTable.xlsx
+++ b/LDMP/data/CarbonSummaryTable.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azvol\Code\LandDegradation\trends.earth\LDMP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAF4D36-6893-4FCC-A79D-AD515861C988}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0065B918-D95E-4CC0-8BCE-1C749721C488}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SDG 15.3.1" sheetId="5" r:id="rId1"/>
+    <sheet name="Total Carbon Summary Table" sheetId="5" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
@@ -89,18 +89,9 @@
     <t>Total carbon emissions over period (tonnes of CO2 equivalent):</t>
   </si>
   <si>
-    <t>Percent of total land area</t>
-  </si>
-  <si>
     <t>Area (hectares)</t>
   </si>
   <si>
-    <t>Forest area:</t>
-  </si>
-  <si>
-    <t>Non-forest land area:</t>
-  </si>
-  <si>
     <t>Water area:</t>
   </si>
   <si>
@@ -108,6 +99,15 @@
   </si>
   <si>
     <t>Total area:</t>
+  </si>
+  <si>
+    <t>Percent of total area</t>
+  </si>
+  <si>
+    <t>Initial forest area:</t>
+  </si>
+  <si>
+    <t>Initial non-forest land area:</t>
   </si>
 </sst>
 </file>
@@ -324,6 +324,39 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -341,39 +374,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="37" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -707,18 +707,19 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="14" customWidth="1"/>
-    <col min="5" max="6" width="15.7109375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="14" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" style="6" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
@@ -737,69 +738,81 @@
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:6" s="16" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:6" s="16" customFormat="1" ht="30.75" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="18"/>
       <c r="C5" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
-      <c r="B6" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="48"/>
+      <c r="B6" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="39"/>
+      <c r="D6" s="40" t="e">
+        <f>C6/$C$10</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="7" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
-      <c r="B7" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="48"/>
+      <c r="B7" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="41"/>
+      <c r="D7" s="40" t="e">
+        <f t="shared" ref="D7:D9" si="0">C7/$C$10</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="8" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
-      <c r="B8" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="48"/>
+      <c r="B8" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="41"/>
+      <c r="D8" s="40" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="9" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
-      <c r="B9" s="43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="45"/>
-      <c r="D9" s="48"/>
+      <c r="B9" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="40" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="10" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="44">
+        <v>17</v>
+      </c>
+      <c r="C10" s="38">
         <f>SUM(C6:C9)</f>
         <v>0</v>
       </c>
-      <c r="D10" s="47"/>
+      <c r="D10" s="37"/>
     </row>
     <row r="11" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
@@ -810,12 +823,12 @@
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="42">
-        <f>SUM(C19:C36)</f>
+      <c r="C12" s="46"/>
+      <c r="D12" s="35">
+        <f>SUM(C19:C38)</f>
         <v>0</v>
       </c>
       <c r="E12" s="23"/>
@@ -823,12 +836,12 @@
     </row>
     <row r="13" spans="1:6" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="42">
-        <f>SUM(F18:F36)</f>
+      <c r="C13" s="46"/>
+      <c r="D13" s="35">
+        <f>SUM(F18:F38)</f>
         <v>0</v>
       </c>
       <c r="E13" s="23"/>
@@ -837,14 +850,14 @@
       <c r="A14" s="1"/>
     </row>
     <row r="15" spans="1:6" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
     </row>
     <row r="16" spans="1:6" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
@@ -877,381 +890,435 @@
     <row r="18" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
       <c r="B18" s="27"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
     </row>
     <row r="19" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
-      <c r="B19" s="27">
-        <f>B18+C19</f>
-        <v>0</v>
-      </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="39">
-        <f>D18+E19</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="41"/>
-      <c r="F19" s="40">
-        <f t="shared" ref="F19:F36" si="0">-E19*3.67</f>
-        <v>0</v>
+      <c r="B19" s="27" t="str">
+        <f>IF(ISBLANK(C19),"",B18+C19)</f>
+        <v/>
+      </c>
+      <c r="C19" s="33"/>
+      <c r="D19" s="32" t="str">
+        <f>IF(ISBLANK(C19),"",D18+E19)</f>
+        <v/>
+      </c>
+      <c r="E19" s="34"/>
+      <c r="F19" s="33" t="str">
+        <f>IF(ISBLANK(E19),"",-E19*3.67)</f>
+        <v/>
       </c>
       <c r="H19" s="28"/>
     </row>
     <row r="20" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
-      <c r="B20" s="27">
-        <f t="shared" ref="B20:B24" si="1">B19+C20</f>
-        <v>0</v>
-      </c>
-      <c r="C20" s="40"/>
-      <c r="D20" s="39">
-        <f t="shared" ref="D20:D34" si="2">D19+E20</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="41"/>
-      <c r="F20" s="40">
-        <f t="shared" ref="F20:F24" si="3">-E20*3.67</f>
-        <v>0</v>
+      <c r="B20" s="27" t="str">
+        <f t="shared" ref="B20:B38" si="1">IF(ISBLANK(C20),"",B19+C20)</f>
+        <v/>
+      </c>
+      <c r="C20" s="33"/>
+      <c r="D20" s="32" t="str">
+        <f t="shared" ref="D20:D38" si="2">IF(ISBLANK(C20),"",D19+E20)</f>
+        <v/>
+      </c>
+      <c r="E20" s="34"/>
+      <c r="F20" s="33" t="str">
+        <f t="shared" ref="F20:F38" si="3">IF(ISBLANK(E20),"",-E20*3.67)</f>
+        <v/>
       </c>
       <c r="G20" s="30"/>
       <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
-      <c r="B21" s="27">
+      <c r="B21" s="27" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="39">
+        <v/>
+      </c>
+      <c r="C21" s="33"/>
+      <c r="D21" s="32" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="41"/>
-      <c r="F21" s="40">
+        <v/>
+      </c>
+      <c r="E21" s="34"/>
+      <c r="F21" s="33" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26"/>
-      <c r="B22" s="27">
+      <c r="B22" s="27" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="39">
+        <v/>
+      </c>
+      <c r="C22" s="33"/>
+      <c r="D22" s="32" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="41"/>
-      <c r="F22" s="40">
+        <v/>
+      </c>
+      <c r="E22" s="34"/>
+      <c r="F22" s="33" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="H22" s="15"/>
     </row>
     <row r="23" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
-      <c r="B23" s="27">
+      <c r="B23" s="27" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="39">
+        <v/>
+      </c>
+      <c r="C23" s="33"/>
+      <c r="D23" s="32" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E23" s="41"/>
-      <c r="F23" s="40">
+        <v/>
+      </c>
+      <c r="E23" s="34"/>
+      <c r="F23" s="33" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
-      <c r="B24" s="27">
+      <c r="B24" s="27" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="39">
+        <v/>
+      </c>
+      <c r="C24" s="33"/>
+      <c r="D24" s="32" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="40">
+        <v/>
+      </c>
+      <c r="E24" s="34"/>
+      <c r="F24" s="33" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="H24" s="15"/>
     </row>
     <row r="25" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
-      <c r="B25" s="27">
-        <f t="shared" ref="B25:B34" si="4">B24+C25</f>
-        <v>0</v>
-      </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="39">
+      <c r="B25" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C25" s="33"/>
+      <c r="D25" s="32" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="41"/>
-      <c r="F25" s="40">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="E25" s="34"/>
+      <c r="F25" s="33" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="H25" s="15"/>
     </row>
     <row r="26" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
-      <c r="B26" s="27">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="39">
+      <c r="B26" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C26" s="33"/>
+      <c r="D26" s="32" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="40">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="E26" s="34"/>
+      <c r="F26" s="33" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="H26" s="15"/>
     </row>
     <row r="27" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
-      <c r="B27" s="27">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="39">
+      <c r="B27" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C27" s="33"/>
+      <c r="D27" s="32" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="41"/>
-      <c r="F27" s="40">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="E27" s="34"/>
+      <c r="F27" s="33" t="str">
+        <f t="shared" si="3"/>
+        <v/>
       </c>
       <c r="H27" s="15"/>
     </row>
     <row r="28" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="40"/>
+      <c r="B28" s="27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C28" s="33"/>
+      <c r="D28" s="32" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="E28" s="34"/>
+      <c r="F28" s="33" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
-      <c r="B29" s="27">
-        <f>B27+C29</f>
-        <v>0</v>
-      </c>
-      <c r="C29" s="40"/>
-      <c r="D29" s="39">
-        <f>D27+E29</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="41"/>
-      <c r="F29" s="40">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="B29" s="27" t="str">
+        <f t="shared" ref="B29:B38" si="4">IF(ISBLANK(C29),"",B28+C29)</f>
+        <v/>
+      </c>
+      <c r="C29" s="33"/>
+      <c r="D29" s="32" t="str">
+        <f t="shared" ref="D29:D38" si="5">IF(ISBLANK(C29),"",D28+E29)</f>
+        <v/>
+      </c>
+      <c r="E29" s="34"/>
+      <c r="F29" s="33" t="str">
+        <f t="shared" ref="F29:F38" si="6">IF(ISBLANK(E29),"",-E29*3.67)</f>
+        <v/>
       </c>
       <c r="H29" s="15"/>
     </row>
-    <row r="30" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
-      <c r="B30" s="27">
+      <c r="B30" s="27" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E30" s="41"/>
-      <c r="F30" s="40">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="C30" s="33"/>
+      <c r="D30" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E30" s="34"/>
+      <c r="F30" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="H30" s="15"/>
     </row>
-    <row r="31" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="26"/>
-      <c r="B31" s="27">
+      <c r="B31" s="27" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="C31" s="40"/>
-      <c r="D31" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E31" s="41"/>
-      <c r="F31" s="40">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="C31" s="33"/>
+      <c r="D31" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E31" s="34"/>
+      <c r="F31" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
-      <c r="B32" s="27">
+      <c r="B32" s="27" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="C32" s="40"/>
-      <c r="D32" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E32" s="41"/>
-      <c r="F32" s="40">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="C32" s="33"/>
+      <c r="D32" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E32" s="34"/>
+      <c r="F32" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="H32" s="15"/>
     </row>
     <row r="33" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="26"/>
-      <c r="B33" s="27">
+      <c r="B33" s="27" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="C33" s="40"/>
-      <c r="D33" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="41"/>
-      <c r="F33" s="40">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="C33" s="33"/>
+      <c r="D33" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E33" s="34"/>
+      <c r="F33" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="H33" s="15"/>
     </row>
     <row r="34" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="26"/>
-      <c r="B34" s="27">
+      <c r="B34" s="27" t="str">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="C34" s="40"/>
-      <c r="D34" s="39">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E34" s="41"/>
-      <c r="F34" s="40">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="C34" s="33"/>
+      <c r="D34" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E34" s="34"/>
+      <c r="F34" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="26"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="40"/>
+      <c r="B35" s="27" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="C35" s="33"/>
+      <c r="D35" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E35" s="34"/>
+      <c r="F35" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
       <c r="H35" s="15"/>
     </row>
     <row r="36" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="26"/>
-      <c r="B36" s="27">
-        <f>B34+C36</f>
+      <c r="B36" s="27" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="C36" s="33"/>
+      <c r="D36" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E36" s="34"/>
+      <c r="F36" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H36" s="15"/>
+    </row>
+    <row r="37" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="26"/>
+      <c r="B37" s="27" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="C37" s="33"/>
+      <c r="D37" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E37" s="34"/>
+      <c r="F37" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H37" s="15"/>
+    </row>
+    <row r="38" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="26"/>
+      <c r="B38" s="27" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="C38" s="33"/>
+      <c r="D38" s="32" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E38" s="34"/>
+      <c r="F38" s="33" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H38" s="15"/>
+    </row>
+    <row r="39" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="19"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="H39" s="15"/>
+    </row>
+    <row r="40" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="45"/>
+      <c r="C40" s="45"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
+    </row>
+    <row r="41" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="21"/>
+      <c r="B41" s="45"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+    </row>
+    <row r="42" spans="1:8" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+    </row>
+    <row r="43" spans="1:8" s="7" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C36" s="40"/>
-      <c r="D36" s="39">
-        <f>D34+E36</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="40">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H36" s="15"/>
-    </row>
-    <row r="37" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="19"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="H37" s="15"/>
-    </row>
-    <row r="38" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-    </row>
-    <row r="39" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-    </row>
-    <row r="40" spans="1:8" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-    </row>
-    <row r="41" spans="1:8" s="7" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-    </row>
-    <row r="43" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
+      <c r="B43" s="44"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="B38:F39"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="B40:F41"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="A43:F43"/>
     <mergeCell ref="A15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add all area calculations.
</commit_message>
<xml_diff>
--- a/LDMP/data/CarbonSummaryTable.xlsx
+++ b/LDMP/data/CarbonSummaryTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azvol\Code\LandDegradation\trends.earth\LDMP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0065B918-D95E-4CC0-8BCE-1C749721C488}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558F9DD9-FDBA-4DE3-909F-60F24F72405F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -260,7 +260,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -336,9 +336,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -356,6 +353,12 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -709,22 +712,22 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="14" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="15.73046875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.73046875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20.73046875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="20.73046875" style="14" customWidth="1"/>
+    <col min="5" max="6" width="20.73046875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="10.86328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -734,21 +737,21 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:6" s="16" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+    <row r="3" spans="1:6" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-    </row>
-    <row r="4" spans="1:6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:6" s="16" customFormat="1" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+    </row>
+    <row r="4" spans="1:6" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="5" spans="1:6" s="16" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="17"/>
       <c r="B5" s="18"/>
       <c r="C5" s="10" t="s">
@@ -759,107 +762,107 @@
       </c>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="9"/>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="40" t="e">
+      <c r="C6" s="38"/>
+      <c r="D6" s="39" t="e">
         <f>C6/$C$10</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="9"/>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="40" t="e">
+      <c r="C7" s="40"/>
+      <c r="D7" s="39" t="e">
         <f t="shared" ref="D7:D9" si="0">C7/$C$10</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="9"/>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="41"/>
-      <c r="D8" s="40" t="e">
+      <c r="C8" s="40"/>
+      <c r="D8" s="39" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="9"/>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="40" t="e">
+      <c r="C9" s="38"/>
+      <c r="D9" s="39" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="9"/>
       <c r="B10" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="37">
         <f>SUM(C6:C9)</f>
         <v>0</v>
       </c>
-      <c r="D10" s="37"/>
-    </row>
-    <row r="11" spans="1:6" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D10" s="36"/>
+    </row>
+    <row r="11" spans="1:6" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="9"/>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
       <c r="D11" s="24"/>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1"/>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="35">
+      <c r="C12" s="47"/>
+      <c r="D12" s="41">
         <f>SUM(C19:C38)</f>
         <v>0</v>
       </c>
       <c r="E12" s="23"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="19" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="20"/>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="35">
+      <c r="C13" s="47"/>
+      <c r="D13" s="41">
         <f>SUM(F18:F38)</f>
         <v>0</v>
       </c>
       <c r="E13" s="23"/>
     </row>
-    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:6" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="47" t="s">
+    <row r="15" spans="1:6" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-    </row>
-    <row r="16" spans="1:6" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+    </row>
+    <row r="16" spans="1:6" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -867,11 +870,11 @@
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="1:8" s="13" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="13" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="42" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="25" t="s">
@@ -887,7 +890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="26"/>
       <c r="B18" s="27"/>
       <c r="C18" s="31"/>
@@ -895,7 +898,7 @@
       <c r="E18" s="31"/>
       <c r="F18" s="31"/>
     </row>
-    <row r="19" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="26"/>
       <c r="B19" s="27" t="str">
         <f>IF(ISBLANK(C19),"",B18+C19)</f>
@@ -913,26 +916,26 @@
       </c>
       <c r="H19" s="28"/>
     </row>
-    <row r="20" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="26"/>
       <c r="B20" s="27" t="str">
-        <f t="shared" ref="B20:B38" si="1">IF(ISBLANK(C20),"",B19+C20)</f>
+        <f t="shared" ref="B20:B28" si="1">IF(ISBLANK(C20),"",B19+C20)</f>
         <v/>
       </c>
       <c r="C20" s="33"/>
       <c r="D20" s="32" t="str">
-        <f t="shared" ref="D20:D38" si="2">IF(ISBLANK(C20),"",D19+E20)</f>
+        <f t="shared" ref="D20:D28" si="2">IF(ISBLANK(C20),"",D19+E20)</f>
         <v/>
       </c>
       <c r="E20" s="34"/>
       <c r="F20" s="33" t="str">
-        <f t="shared" ref="F20:F38" si="3">IF(ISBLANK(E20),"",-E20*3.67)</f>
+        <f t="shared" ref="F20:F28" si="3">IF(ISBLANK(E20),"",-E20*3.67)</f>
         <v/>
       </c>
       <c r="G20" s="30"/>
       <c r="H20" s="15"/>
     </row>
-    <row r="21" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="26"/>
       <c r="B21" s="27" t="str">
         <f t="shared" si="1"/>
@@ -950,7 +953,7 @@
       </c>
       <c r="H21" s="15"/>
     </row>
-    <row r="22" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="26"/>
       <c r="B22" s="27" t="str">
         <f t="shared" si="1"/>
@@ -968,7 +971,7 @@
       </c>
       <c r="H22" s="15"/>
     </row>
-    <row r="23" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="26"/>
       <c r="B23" s="27" t="str">
         <f t="shared" si="1"/>
@@ -986,7 +989,7 @@
       </c>
       <c r="H23" s="15"/>
     </row>
-    <row r="24" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="26"/>
       <c r="B24" s="27" t="str">
         <f t="shared" si="1"/>
@@ -1004,7 +1007,7 @@
       </c>
       <c r="H24" s="15"/>
     </row>
-    <row r="25" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="26"/>
       <c r="B25" s="27" t="str">
         <f t="shared" si="1"/>
@@ -1022,7 +1025,7 @@
       </c>
       <c r="H25" s="15"/>
     </row>
-    <row r="26" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="26"/>
       <c r="B26" s="27" t="str">
         <f t="shared" si="1"/>
@@ -1040,7 +1043,7 @@
       </c>
       <c r="H26" s="15"/>
     </row>
-    <row r="27" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A27" s="26"/>
       <c r="B27" s="27" t="str">
         <f t="shared" si="1"/>
@@ -1058,7 +1061,7 @@
       </c>
       <c r="H27" s="15"/>
     </row>
-    <row r="28" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="26"/>
       <c r="B28" s="27" t="str">
         <f t="shared" si="1"/>
@@ -1076,7 +1079,7 @@
       </c>
       <c r="H28" s="15"/>
     </row>
-    <row r="29" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A29" s="26"/>
       <c r="B29" s="27" t="str">
         <f t="shared" ref="B29:B38" si="4">IF(ISBLANK(C29),"",B28+C29)</f>
@@ -1094,7 +1097,7 @@
       </c>
       <c r="H29" s="15"/>
     </row>
-    <row r="30" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A30" s="26"/>
       <c r="B30" s="27" t="str">
         <f t="shared" si="4"/>
@@ -1112,7 +1115,7 @@
       </c>
       <c r="H30" s="15"/>
     </row>
-    <row r="31" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A31" s="26"/>
       <c r="B31" s="27" t="str">
         <f t="shared" si="4"/>
@@ -1130,7 +1133,7 @@
       </c>
       <c r="H31" s="15"/>
     </row>
-    <row r="32" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A32" s="26"/>
       <c r="B32" s="27" t="str">
         <f t="shared" si="4"/>
@@ -1148,7 +1151,7 @@
       </c>
       <c r="H32" s="15"/>
     </row>
-    <row r="33" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A33" s="26"/>
       <c r="B33" s="27" t="str">
         <f t="shared" si="4"/>
@@ -1166,7 +1169,7 @@
       </c>
       <c r="H33" s="15"/>
     </row>
-    <row r="34" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A34" s="26"/>
       <c r="B34" s="27" t="str">
         <f t="shared" si="4"/>
@@ -1184,7 +1187,7 @@
       </c>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="26"/>
       <c r="B35" s="27" t="str">
         <f t="shared" si="4"/>
@@ -1202,7 +1205,7 @@
       </c>
       <c r="H35" s="15"/>
     </row>
-    <row r="36" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A36" s="26"/>
       <c r="B36" s="27" t="str">
         <f t="shared" si="4"/>
@@ -1220,7 +1223,7 @@
       </c>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="26"/>
       <c r="B37" s="27" t="str">
         <f t="shared" si="4"/>
@@ -1238,7 +1241,7 @@
       </c>
       <c r="H37" s="15"/>
     </row>
-    <row r="38" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A38" s="26"/>
       <c r="B38" s="27" t="str">
         <f t="shared" si="4"/>
@@ -1256,7 +1259,7 @@
       </c>
       <c r="H38" s="15"/>
     </row>
-    <row r="39" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A39" s="19"/>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
@@ -1265,25 +1268,25 @@
       <c r="F39" s="22"/>
       <c r="H39" s="15"/>
     </row>
-    <row r="40" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B40" s="45"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-    </row>
-    <row r="41" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="46"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+    </row>
+    <row r="41" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A41" s="21"/>
-      <c r="B41" s="45"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
-    </row>
-    <row r="42" spans="1:8" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+    </row>
+    <row r="42" spans="1:8" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1"/>
       <c r="B42" s="11"/>
       <c r="C42" s="12"/>
@@ -1291,25 +1294,25 @@
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
     </row>
-    <row r="43" spans="1:8" s="7" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="44" t="s">
+    <row r="43" spans="1:8" s="7" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="44"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="44" t="s">
+      <c r="B43" s="45"/>
+      <c r="C43" s="45"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A45" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="44"/>
-      <c r="C45" s="44"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>